<commit_message>
"sua lai loi nhap so am"
</commit_message>
<xml_diff>
--- a/Prj2/java/DAO/QLTuThuoc.xlsx
+++ b/Prj2/java/DAO/QLTuThuoc.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357776" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357890" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>150ml 1 ngày</t>
+  </si>
+  <si>
+    <t>Acemol1</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="92">
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
@@ -343,6 +346,10 @@
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
@@ -698,7 +705,7 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="86" t="n">
+      <c r="F2" s="90" t="n">
         <v>45005.0</v>
       </c>
     </row>
@@ -718,7 +725,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="86" t="n">
+      <c r="F3" s="90" t="n">
         <v>44757.0</v>
       </c>
     </row>
@@ -738,7 +745,7 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="86" t="n">
+      <c r="F4" s="90" t="n">
         <v>45000.0</v>
       </c>
     </row>
@@ -758,7 +765,7 @@
       <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="86" t="n">
+      <c r="F5" s="90" t="n">
         <v>45119.0</v>
       </c>
     </row>
@@ -778,8 +785,8 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="86" t="n">
-        <v>44760.0</v>
+      <c r="F6" s="90" t="n">
+        <v>44779.0</v>
       </c>
     </row>
     <row r="7">
@@ -798,7 +805,7 @@
       <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="86" t="n">
+      <c r="F7" s="90" t="n">
         <v>37467.0</v>
       </c>
     </row>
@@ -818,7 +825,7 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="86" t="n">
+      <c r="F8" s="90" t="n">
         <v>37467.0</v>
       </c>
     </row>
@@ -838,7 +845,7 @@
       <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="86" t="n">
+      <c r="F9" s="90" t="n">
         <v>45000.0</v>
       </c>
     </row>
@@ -858,7 +865,7 @@
       <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="86" t="n">
+      <c r="F10" s="90" t="n">
         <v>37467.0</v>
       </c>
     </row>
@@ -878,7 +885,7 @@
       <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="86" t="n">
+      <c r="F11" s="90" t="n">
         <v>45005.0</v>
       </c>
     </row>
@@ -898,7 +905,7 @@
       <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="86" t="n">
+      <c r="F12" s="90" t="n">
         <v>44772.0</v>
       </c>
     </row>
@@ -946,10 +953,10 @@
       <c r="B2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="n" s="87">
+      <c r="C2" t="n" s="91">
         <v>44757.0</v>
       </c>
-      <c r="D2" t="n" s="87">
+      <c r="D2" t="n" s="91">
         <v>44755.0</v>
       </c>
     </row>
@@ -960,10 +967,10 @@
       <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="C3" t="n" s="87">
+      <c r="C3" t="n" s="91">
         <v>44751.0</v>
       </c>
-      <c r="D3" t="n" s="87">
+      <c r="D3" t="n" s="91">
         <v>44745.0</v>
       </c>
     </row>
@@ -974,10 +981,10 @@
       <c r="B4" t="s">
         <v>79</v>
       </c>
-      <c r="C4" t="n" s="87">
+      <c r="C4" t="n" s="91">
         <v>44761.0</v>
       </c>
-      <c r="D4" t="n" s="87">
+      <c r="D4" t="n" s="91">
         <v>44757.0</v>
       </c>
     </row>

</xml_diff>